<commit_message>
factor_backtest: calculate hold weight first, support holdday; backtest from wight is not supported yet
</commit_message>
<xml_diff>
--- a/factor_backtest/factors_tested.xlsx
+++ b/factor_backtest/factors_tested.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\factor_backtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56A8E42-62F9-4119-A664-04F2AD794A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E467D32F-26C8-447D-8688-FB4E03EE5B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4116" yWindow="2136" windowWidth="11484" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>

</xml_diff>